<commit_message>
import thêm mới sản phẩm sai nhóm hàng
</commit_message>
<xml_diff>
--- a/CAP_TEAM05_2022/Uploads/Mau_Nhap_Lieu (5).xlsx
+++ b/CAP_TEAM05_2022/Uploads/Mau_Nhap_Lieu (5).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A30A6C-A3BE-44AE-8CA1-3EF864CB71AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C37D59D-4F21-4347-A781-23A0EC22240F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>Tên sản phẩm</t>
   </si>
@@ -62,10 +62,25 @@
     <t>Phân bón fail fail</t>
   </si>
   <si>
-    <t>Sai nhóm hàng</t>
-  </si>
-  <si>
     <t>Sai rồi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phân bón fail fail 2 </t>
+  </si>
+  <si>
+    <t>Công ty Adama</t>
+  </si>
+  <si>
+    <t>sai rồi nè 3</t>
+  </si>
+  <si>
+    <t>sai nữa nè 3</t>
+  </si>
+  <si>
+    <t>sai nữa nè 5</t>
+  </si>
+  <si>
+    <t>sai rồi nè 5</t>
   </si>
 </sst>
 </file>
@@ -463,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,10 +519,10 @@
         <v>8</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>10</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>7</v>
@@ -519,6 +534,75 @@
         <v>18000</v>
       </c>
       <c r="G2" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1">
+        <v>50000</v>
+      </c>
+      <c r="F3" s="1">
+        <v>18000</v>
+      </c>
+      <c r="G3" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1">
+        <v>50000</v>
+      </c>
+      <c r="F4" s="1">
+        <v>18000</v>
+      </c>
+      <c r="G4" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1">
+        <v>50000</v>
+      </c>
+      <c r="F5" s="1">
+        <v>18000</v>
+      </c>
+      <c r="G5" s="1">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cập nhật import fails
</commit_message>
<xml_diff>
--- a/CAP_TEAM05_2022/Uploads/Mau_Nhap_Lieu (5).xlsx
+++ b/CAP_TEAM05_2022/Uploads/Mau_Nhap_Lieu (5).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C37D59D-4F21-4347-A781-23A0EC22240F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F5CCE2-C2C5-4E78-8374-71E852E3CEF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Tên sản phẩm</t>
   </si>
@@ -71,16 +71,22 @@
     <t>Công ty Adama</t>
   </si>
   <si>
+    <t>sai rồi nè 1</t>
+  </si>
+  <si>
+    <t>sai nữa nè 2</t>
+  </si>
+  <si>
     <t>sai rồi nè 3</t>
   </si>
   <si>
-    <t>sai nữa nè 3</t>
-  </si>
-  <si>
-    <t>sai nữa nè 5</t>
-  </si>
-  <si>
-    <t>sai rồi nè 5</t>
+    <t>sai nữa nè 4</t>
+  </si>
+  <si>
+    <t>Phân bón fail fail 3</t>
+  </si>
+  <si>
+    <t>Phân bón fail fail 4</t>
   </si>
 </sst>
 </file>
@@ -481,7 +487,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -562,10 +568,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>9</v>
@@ -585,13 +591,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>7</v>

</xml_diff>